<commit_message>
Changed GPA as number
</commit_message>
<xml_diff>
--- a/Cleaned-Data/2016-Passouts/Sem-3_2016_Passout_cleaned.xlsx
+++ b/Cleaned-Data/2016-Passouts/Sem-3_2016_Passout_cleaned.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prashant/Downloads/Student-Placement-Guidance/Cleaned-Data/2016-Passouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tejas\Student-Placement-Guidance\Cleaned-Data\2016-Passouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15920"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15915"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="200">
   <si>
     <t>M3-TH</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>--</t>
   </si>
   <si>
     <t>P</t>
@@ -638,7 +635,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1126,38 +1123,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.796875" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="22.83203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.19921875" customWidth="1"/>
-    <col min="23" max="23" width="4.3984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.1640625" customWidth="1"/>
+    <col min="23" max="23" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1166,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -1181,10 +1178,10 @@
         <v>6</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>5</v>
@@ -1193,10 +1190,10 @@
         <v>7</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>8</v>
@@ -1205,10 +1202,10 @@
         <v>9</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>197</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>10</v>
@@ -1217,18 +1214,18 @@
         <v>11</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="W1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="X1" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="X1" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="11">
         <v>233201</v>
@@ -1296,13 +1293,13 @@
       <c r="W2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="11">
         <v>233202</v>
@@ -1370,14 +1367,14 @@
       <c r="W3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="7" t="s">
-        <v>13</v>
+      <c r="X3" s="7">
+        <v>0</v>
       </c>
       <c r="Y3" s="7"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="11">
         <v>233203</v>
@@ -1445,13 +1442,13 @@
       <c r="W4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="11">
         <v>233204</v>
@@ -1517,15 +1514,15 @@
         <v>23</v>
       </c>
       <c r="W5" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X5" s="7">
         <v>6.64</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="11">
         <v>233205</v>
@@ -1591,15 +1588,15 @@
         <v>23</v>
       </c>
       <c r="W6" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X6" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="11">
         <v>233206</v>
@@ -1667,13 +1664,13 @@
       <c r="W7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X7" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="11">
         <v>233207</v>
@@ -1741,13 +1738,13 @@
       <c r="W8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X8" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="11">
         <v>233208</v>
@@ -1815,13 +1812,13 @@
       <c r="W9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X9" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="11">
         <v>233209</v>
@@ -1887,15 +1884,15 @@
         <v>22</v>
       </c>
       <c r="W10" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X10" s="7">
         <v>6.86</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="11">
         <v>233210</v>
@@ -1963,13 +1960,13 @@
       <c r="W11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X11" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B12" s="11">
         <v>233363</v>
@@ -2037,13 +2034,13 @@
       <c r="W12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X12" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="11">
         <v>233211</v>
@@ -2111,13 +2108,13 @@
       <c r="W13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X13" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="11">
         <v>233212</v>
@@ -2185,13 +2182,13 @@
       <c r="W14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X14" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="11">
         <v>233213</v>
@@ -2259,13 +2256,13 @@
       <c r="W15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X15" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="X15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="11">
         <v>233214</v>
@@ -2331,15 +2328,15 @@
         <v>24</v>
       </c>
       <c r="W16" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X16" s="7">
         <v>7.32</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="11">
         <v>233215</v>
@@ -2407,13 +2404,13 @@
       <c r="W17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X17" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="11">
         <v>233216</v>
@@ -2479,15 +2476,15 @@
         <v>20</v>
       </c>
       <c r="W18" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X18" s="7">
         <v>6.96</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="11">
         <v>233217</v>
@@ -2553,15 +2550,15 @@
         <v>22</v>
       </c>
       <c r="W19" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X19" s="7">
         <v>7.54</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="11">
         <v>233218</v>
@@ -2629,13 +2626,13 @@
       <c r="W20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X20" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="11">
         <v>233219</v>
@@ -2701,15 +2698,15 @@
         <v>23</v>
       </c>
       <c r="W21" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X21" s="7">
         <v>6.89</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="11">
         <v>233220</v>
@@ -2777,13 +2774,13 @@
       <c r="W22" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X22" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X22" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="11">
         <v>233221</v>
@@ -2851,13 +2848,13 @@
       <c r="W23" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X23" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X23" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="11">
         <v>233222</v>
@@ -2925,13 +2922,13 @@
       <c r="W24" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X24" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="11">
         <v>233223</v>
@@ -2999,13 +2996,13 @@
       <c r="W25" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X25" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="11">
         <v>233224</v>
@@ -3071,15 +3068,15 @@
         <v>21</v>
       </c>
       <c r="W26" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X26" s="7">
         <v>7.71</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="11">
         <v>233225</v>
@@ -3145,15 +3142,15 @@
         <v>23</v>
       </c>
       <c r="W27" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X27" s="7">
         <v>7.43</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="11">
         <v>233226</v>
@@ -3219,15 +3216,15 @@
         <v>20</v>
       </c>
       <c r="W28" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X28" s="7">
         <v>6.46</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="11">
         <v>233227</v>
@@ -3293,15 +3290,15 @@
         <v>24</v>
       </c>
       <c r="W29" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X29" s="7">
         <v>6.57</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="11">
         <v>233228</v>
@@ -3367,15 +3364,15 @@
         <v>20</v>
       </c>
       <c r="W30" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X30" s="7">
         <v>6.68</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="11">
         <v>233229</v>
@@ -3443,16 +3440,16 @@
       <c r="W31" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X31" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X31" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>187</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>188</v>
       </c>
       <c r="C32" s="6">
         <v>1</v>
@@ -3517,13 +3514,13 @@
       <c r="W32" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X32" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="11">
         <v>233230</v>
@@ -3591,13 +3588,13 @@
       <c r="W33" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X33" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="11">
         <v>233231</v>
@@ -3665,13 +3662,13 @@
       <c r="W34" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X34" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X34" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" s="11">
         <v>233232</v>
@@ -3737,15 +3734,15 @@
         <v>20</v>
       </c>
       <c r="W35" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X35" s="7">
         <v>7.25</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B36" s="11">
         <v>233233</v>
@@ -3811,15 +3808,15 @@
         <v>22</v>
       </c>
       <c r="W36" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X36" s="7">
         <v>7.68</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="11">
         <v>233234</v>
@@ -3887,13 +3884,13 @@
       <c r="W37" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X37" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="11">
         <v>233235</v>
@@ -3961,13 +3958,13 @@
       <c r="W38" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X38" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X38" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="11">
         <v>233236</v>
@@ -4035,13 +4032,13 @@
       <c r="W39" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X39" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="11">
         <v>233237</v>
@@ -4109,13 +4106,13 @@
       <c r="W40" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X40" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X40" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="11">
         <v>233238</v>
@@ -4181,15 +4178,15 @@
         <v>20</v>
       </c>
       <c r="W41" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X41" s="7">
         <v>7.29</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="11">
         <v>233239</v>
@@ -4255,15 +4252,15 @@
         <v>23</v>
       </c>
       <c r="W42" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X42" s="7">
         <v>7.39</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="11">
         <v>233240</v>
@@ -4331,13 +4328,13 @@
       <c r="W43" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X43" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="11">
         <v>233241</v>
@@ -4405,13 +4402,13 @@
       <c r="W44" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X44" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="11">
         <v>233242</v>
@@ -4479,13 +4476,13 @@
       <c r="W45" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X45" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X45" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="11">
         <v>233243</v>
@@ -4551,15 +4548,15 @@
         <v>21</v>
       </c>
       <c r="W46" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X46" s="7">
         <v>8.18</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="11">
         <v>233244</v>
@@ -4627,13 +4624,13 @@
       <c r="W47" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X47" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X47" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="11">
         <v>233245</v>
@@ -4701,13 +4698,13 @@
       <c r="W48" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X48" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X48" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B49" s="11">
         <v>233246</v>
@@ -4773,15 +4770,15 @@
         <v>24</v>
       </c>
       <c r="W49" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X49" s="7">
         <v>8.25</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B50" s="11">
         <v>233247</v>
@@ -4847,15 +4844,15 @@
         <v>24</v>
       </c>
       <c r="W50" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X50" s="7">
         <v>6.11</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" s="11">
         <v>233248</v>
@@ -4923,13 +4920,13 @@
       <c r="W51" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X51" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X51" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="11">
         <v>233249</v>
@@ -4995,15 +4992,15 @@
         <v>23</v>
       </c>
       <c r="W52" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X52" s="7">
         <v>6.79</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" s="11">
         <v>233250</v>
@@ -5071,13 +5068,13 @@
       <c r="W53" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X53" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X53" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B54" s="11">
         <v>233251</v>
@@ -5143,15 +5140,15 @@
         <v>24</v>
       </c>
       <c r="W54" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X54" s="7">
         <v>6.93</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B55" s="11">
         <v>233252</v>
@@ -5219,13 +5216,13 @@
       <c r="W55" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X55" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X55" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B56" s="11">
         <v>233253</v>
@@ -5291,15 +5288,15 @@
         <v>23</v>
       </c>
       <c r="W56" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X56" s="7">
         <v>7.57</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B57" s="11">
         <v>233254</v>
@@ -5365,15 +5362,15 @@
         <v>22</v>
       </c>
       <c r="W57" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X57" s="7">
         <v>7.21</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B58" s="11">
         <v>233255</v>
@@ -5441,13 +5438,13 @@
       <c r="W58" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X58" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X58" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B59" s="11">
         <v>233256</v>
@@ -5515,13 +5512,13 @@
       <c r="W59" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X59" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X59" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B60" s="11">
         <v>233257</v>
@@ -5587,15 +5584,15 @@
         <v>22</v>
       </c>
       <c r="W60" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X60" s="7">
         <v>7.82</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B61" s="11">
         <v>233258</v>
@@ -5661,15 +5658,15 @@
         <v>23</v>
       </c>
       <c r="W61" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X61" s="7">
         <v>8.07</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" s="11">
         <v>233259</v>
@@ -5737,13 +5734,13 @@
       <c r="W62" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X62" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X62" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B63" s="11">
         <v>233260</v>
@@ -5811,13 +5808,13 @@
       <c r="W63" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X63" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X63" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B64" s="11">
         <v>233261</v>
@@ -5883,15 +5880,15 @@
         <v>23</v>
       </c>
       <c r="W64" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X64" s="7">
         <v>6.71</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" s="11">
         <v>233262</v>
@@ -5957,15 +5954,15 @@
         <v>22</v>
       </c>
       <c r="W65" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X65" s="7">
         <v>8.25</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" s="11">
         <v>233263</v>
@@ -6033,13 +6030,13 @@
       <c r="W66" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X66" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X66" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A67" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67" s="11">
         <v>233264</v>
@@ -6105,15 +6102,15 @@
         <v>20</v>
       </c>
       <c r="W67" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X67" s="7">
         <v>6.32</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A68" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" s="11">
         <v>233265</v>
@@ -6179,15 +6176,15 @@
         <v>20</v>
       </c>
       <c r="W68" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X68" s="7">
         <v>6.29</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69" s="11">
         <v>233266</v>
@@ -6253,15 +6250,15 @@
         <v>19</v>
       </c>
       <c r="W69" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X69" s="7">
         <v>6.64</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" s="11">
         <v>233267</v>
@@ -6329,13 +6326,13 @@
       <c r="W70" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X70" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X70" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B71" s="11">
         <v>233268</v>
@@ -6403,13 +6400,13 @@
       <c r="W71" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X71" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X71" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B72" s="11">
         <v>233269</v>
@@ -6475,15 +6472,15 @@
         <v>20</v>
       </c>
       <c r="W72" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X72" s="7">
         <v>6.21</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A73" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B73" s="11">
         <v>233270</v>
@@ -6551,13 +6548,13 @@
       <c r="W73" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X73" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X73" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B74" s="11">
         <v>233271</v>
@@ -6625,13 +6622,13 @@
       <c r="W74" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X74" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X74" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B75" s="11">
         <v>233272</v>
@@ -6697,15 +6694,15 @@
         <v>23</v>
       </c>
       <c r="W75" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X75" s="7">
         <v>6.14</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A76" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B76" s="11">
         <v>233273</v>
@@ -6773,13 +6770,13 @@
       <c r="W76" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X76" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X76" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B77" s="11">
         <v>233274</v>
@@ -6845,15 +6842,15 @@
         <v>20</v>
       </c>
       <c r="W77" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X77" s="7">
         <v>6.89</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A78" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B78" s="11">
         <v>233275</v>
@@ -6921,13 +6918,13 @@
       <c r="W78" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X78" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X78" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A79" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B79" s="11">
         <v>233276</v>
@@ -6995,13 +6992,13 @@
       <c r="W79" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X79" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X79" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A80" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B80" s="11">
         <v>233277</v>
@@ -7069,16 +7066,16 @@
       <c r="W80" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X80" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X80" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B81" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="C81" s="6">
         <v>1</v>
@@ -7143,13 +7140,13 @@
       <c r="W81" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X81" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X81" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B82" s="11">
         <v>233278</v>
@@ -7217,13 +7214,13 @@
       <c r="W82" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X82" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X82" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B83" s="11">
         <v>233279</v>
@@ -7291,13 +7288,13 @@
       <c r="W83" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X83" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X83" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B84" s="11">
         <v>233280</v>
@@ -7365,13 +7362,13 @@
       <c r="W84" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X84" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X84" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B85" s="11">
         <v>233281</v>
@@ -7439,13 +7436,13 @@
       <c r="W85" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X85" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X85" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B86" s="11">
         <v>233282</v>
@@ -7513,13 +7510,13 @@
       <c r="W86" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X86" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X86" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B87" s="11">
         <v>233365</v>
@@ -7587,13 +7584,13 @@
       <c r="W87" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X87" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X87" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B88" s="11">
         <v>233283</v>
@@ -7661,13 +7658,13 @@
       <c r="W88" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X88" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X88" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B89" s="11">
         <v>233284</v>
@@ -7733,15 +7730,15 @@
         <v>20</v>
       </c>
       <c r="W89" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X89" s="7">
         <v>6.32</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B90" s="11">
         <v>233285</v>
@@ -7809,13 +7806,13 @@
       <c r="W90" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X90" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X90" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B91" s="11">
         <v>233286</v>
@@ -7881,15 +7878,15 @@
         <v>24</v>
       </c>
       <c r="W91" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X91" s="7">
         <v>8.5399999999999991</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B92" s="11">
         <v>233364</v>
@@ -7957,13 +7954,13 @@
       <c r="W92" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X92" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X92" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B93" s="11">
         <v>233287</v>
@@ -8029,15 +8026,15 @@
         <v>24</v>
       </c>
       <c r="W93" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X93" s="7">
         <v>7.36</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B94" s="11">
         <v>233288</v>
@@ -8105,13 +8102,13 @@
       <c r="W94" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X94" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X94" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B95" s="11">
         <v>233289</v>
@@ -8179,13 +8176,13 @@
       <c r="W95" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X95" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X95" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B96" s="11">
         <v>233290</v>
@@ -8253,13 +8250,13 @@
       <c r="W96" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X96" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X96" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A97" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B97" s="11">
         <v>233291</v>
@@ -8325,15 +8322,15 @@
         <v>21</v>
       </c>
       <c r="W97" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X97" s="7">
         <v>6.82</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A98" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B98" s="11">
         <v>233292</v>
@@ -8401,13 +8398,13 @@
       <c r="W98" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X98" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X98" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A99" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B99" s="11">
         <v>233293</v>
@@ -8475,13 +8472,13 @@
       <c r="W99" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X99" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X99" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A100" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B100" s="11">
         <v>233294</v>
@@ -8549,13 +8546,13 @@
       <c r="W100" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X100" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X100" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A101" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B101" s="11">
         <v>233295</v>
@@ -8623,13 +8620,13 @@
       <c r="W101" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X101" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X101" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A102" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B102" s="11">
         <v>233296</v>
@@ -8697,13 +8694,13 @@
       <c r="W102" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X102" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X102" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A103" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B103" s="11">
         <v>233367</v>
@@ -8769,15 +8766,15 @@
         <v>22</v>
       </c>
       <c r="W103" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X103" s="7">
         <v>6.29</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A104" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B104" s="11">
         <v>233297</v>
@@ -8845,13 +8842,13 @@
       <c r="W104" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X104" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X104" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A105" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B105" s="11">
         <v>233298</v>
@@ -8917,15 +8914,15 @@
         <v>23</v>
       </c>
       <c r="W105" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X105" s="7">
         <v>7.71</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A106" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B106" s="11">
         <v>233299</v>
@@ -8993,13 +8990,13 @@
       <c r="W106" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X106" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X106" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A107" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B107" s="11">
         <v>233300</v>
@@ -9067,13 +9064,13 @@
       <c r="W107" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X107" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X107" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A108" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B108" s="11">
         <v>233301</v>
@@ -9141,13 +9138,13 @@
       <c r="W108" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X108" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X108" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A109" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B109" s="11">
         <v>233302</v>
@@ -9213,15 +9210,15 @@
         <v>23</v>
       </c>
       <c r="W109" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X109" s="7">
         <v>6.71</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A110" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B110" s="11">
         <v>233303</v>
@@ -9289,13 +9286,13 @@
       <c r="W110" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X110" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X110" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A111" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B111" s="11">
         <v>233304</v>
@@ -9363,13 +9360,13 @@
       <c r="W111" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X111" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X111" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A112" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B112" s="11">
         <v>233305</v>
@@ -9435,15 +9432,15 @@
         <v>21</v>
       </c>
       <c r="W112" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X112" s="7">
         <v>8.5399999999999991</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A113" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B113" s="11">
         <v>233306</v>
@@ -9511,13 +9508,13 @@
       <c r="W113" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X113" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X113" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A114" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B114" s="11">
         <v>233307</v>
@@ -9585,13 +9582,13 @@
       <c r="W114" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X114" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X114" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A115" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B115" s="11">
         <v>233308</v>
@@ -9657,15 +9654,15 @@
         <v>24</v>
       </c>
       <c r="W115" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X115" s="7">
         <v>7.79</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A116" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B116" s="11">
         <v>233309</v>
@@ -9731,15 +9728,15 @@
         <v>24</v>
       </c>
       <c r="W116" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X116" s="7">
         <v>7.25</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A117" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B117" s="11">
         <v>233310</v>
@@ -9805,15 +9802,15 @@
         <v>22</v>
       </c>
       <c r="W117" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X117" s="7">
         <v>7.29</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A118" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B118" s="11">
         <v>233311</v>
@@ -9881,13 +9878,13 @@
       <c r="W118" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X118" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X118" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A119" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B119" s="11">
         <v>233312</v>
@@ -9953,15 +9950,15 @@
         <v>20</v>
       </c>
       <c r="W119" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X119" s="7">
         <v>7.79</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A120" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B120" s="11">
         <v>233313</v>
@@ -10029,13 +10026,13 @@
       <c r="W120" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X120" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X120" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A121" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B121" s="11">
         <v>233314</v>
@@ -10103,13 +10100,13 @@
       <c r="W121" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X121" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X121" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A122" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B122" s="11">
         <v>233315</v>
@@ -10175,15 +10172,15 @@
         <v>20</v>
       </c>
       <c r="W122" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X122" s="7">
         <v>6.29</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A123" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B123" s="11">
         <v>233316</v>
@@ -10249,15 +10246,15 @@
         <v>18</v>
       </c>
       <c r="W123" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X123" s="7">
         <v>7.18</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A124" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B124" s="11">
         <v>233371</v>
@@ -10325,13 +10322,13 @@
       <c r="W124" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X124" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X124" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A125" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B125" s="11">
         <v>233317</v>
@@ -10399,13 +10396,13 @@
       <c r="W125" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X125" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X125" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A126" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B126" s="11">
         <v>233318</v>
@@ -10473,13 +10470,13 @@
       <c r="W126" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X126" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X126" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A127" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B127" s="11">
         <v>233319</v>
@@ -10545,15 +10542,15 @@
         <v>21</v>
       </c>
       <c r="W127" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X127" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A128" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B128" s="11">
         <v>233320</v>
@@ -10619,15 +10616,15 @@
         <v>24</v>
       </c>
       <c r="W128" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X128" s="7">
         <v>7.54</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A129" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B129" s="11">
         <v>233321</v>
@@ -10695,13 +10692,13 @@
       <c r="W129" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X129" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X129" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A130" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B130" s="11">
         <v>233322</v>
@@ -10769,13 +10766,13 @@
       <c r="W130" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X130" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X130" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A131" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B131" s="11">
         <v>233323</v>
@@ -10843,13 +10840,13 @@
       <c r="W131" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X131" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X131" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A132" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B132" s="11">
         <v>233324</v>
@@ -10917,13 +10914,13 @@
       <c r="W132" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X132" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X132" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A133" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B133" s="11">
         <v>233325</v>
@@ -10991,13 +10988,13 @@
       <c r="W133" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X133" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X133" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A134" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B134" s="11">
         <v>233326</v>
@@ -11063,15 +11060,15 @@
         <v>24</v>
       </c>
       <c r="W134" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X134" s="7">
         <v>9.7100000000000009</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A135" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B135" s="11">
         <v>233327</v>
@@ -11139,13 +11136,13 @@
       <c r="W135" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X135" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X135" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A136" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B136" s="11">
         <v>233328</v>
@@ -11213,13 +11210,13 @@
       <c r="W136" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X136" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X136" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A137" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B137" s="11">
         <v>233329</v>
@@ -11287,13 +11284,13 @@
       <c r="W137" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X137" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X137" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A138" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B138" s="11">
         <v>233330</v>
@@ -11361,13 +11358,13 @@
       <c r="W138" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X138" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X138" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A139" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B139" s="11">
         <v>233331</v>
@@ -11435,13 +11432,13 @@
       <c r="W139" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X139" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X139" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A140" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B140" s="11">
         <v>233332</v>
@@ -11509,13 +11506,13 @@
       <c r="W140" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X140" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X140" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A141" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B141" s="11">
         <v>233333</v>
@@ -11583,13 +11580,13 @@
       <c r="W141" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X141" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X141" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A142" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B142" s="11">
         <v>233334</v>
@@ -11657,13 +11654,13 @@
       <c r="W142" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X142" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X142" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A143" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B143" s="11">
         <v>233335</v>
@@ -11731,13 +11728,13 @@
       <c r="W143" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X143" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X143" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A144" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B144" s="11">
         <v>233336</v>
@@ -11803,15 +11800,15 @@
         <v>24</v>
       </c>
       <c r="W144" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X144" s="7">
         <v>9.11</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A145" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B145" s="11">
         <v>233337</v>
@@ -11879,13 +11876,13 @@
       <c r="W145" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X145" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X145" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A146" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B146" s="11">
         <v>233338</v>
@@ -11951,15 +11948,15 @@
         <v>21</v>
       </c>
       <c r="W146" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X146" s="7">
         <v>6.86</v>
       </c>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A147" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B147" s="11">
         <v>233339</v>
@@ -12025,15 +12022,15 @@
         <v>24</v>
       </c>
       <c r="W147" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X147" s="7">
         <v>8.36</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A148" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B148" s="11">
         <v>233369</v>
@@ -12101,13 +12098,13 @@
       <c r="W148" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X148" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X148" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A149" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B149" s="11">
         <v>233340</v>
@@ -12175,13 +12172,13 @@
       <c r="W149" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X149" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X149" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A150" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B150" s="11">
         <v>233341</v>
@@ -12249,13 +12246,13 @@
       <c r="W150" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X150" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X150" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A151" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B151" s="11">
         <v>233342</v>
@@ -12321,15 +12318,15 @@
         <v>23</v>
       </c>
       <c r="W151" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X151" s="7">
         <v>8.57</v>
       </c>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A152" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B152" s="11">
         <v>233343</v>
@@ -12397,13 +12394,13 @@
       <c r="W152" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X152" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X152" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A153" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B153" s="11">
         <v>233344</v>
@@ -12471,13 +12468,13 @@
       <c r="W153" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X153" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X153" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A154" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B154" s="11">
         <v>233345</v>
@@ -12545,13 +12542,13 @@
       <c r="W154" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X154" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X154" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A155" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B155" s="11">
         <v>233346</v>
@@ -12619,13 +12616,13 @@
       <c r="W155" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X155" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X155" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A156" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B156" s="11">
         <v>233347</v>
@@ -12693,13 +12690,13 @@
       <c r="W156" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X156" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X156" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A157" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B157" s="11">
         <v>233348</v>
@@ -12767,13 +12764,13 @@
       <c r="W157" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X157" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X157" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A158" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B158" s="11">
         <v>233370</v>
@@ -12839,15 +12836,15 @@
         <v>23</v>
       </c>
       <c r="W158" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X158" s="7">
         <v>6.46</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A159" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B159" s="11">
         <v>233349</v>
@@ -12913,15 +12910,15 @@
         <v>23</v>
       </c>
       <c r="W159" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X159" s="7">
         <v>7.04</v>
       </c>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A160" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B160" s="11">
         <v>233350</v>
@@ -12987,15 +12984,15 @@
         <v>22</v>
       </c>
       <c r="W160" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X160" s="7">
         <v>7.07</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A161" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B161" s="11">
         <v>233351</v>
@@ -13063,13 +13060,13 @@
       <c r="W161" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X161" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X161" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A162" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B162" s="11">
         <v>233352</v>
@@ -13137,13 +13134,13 @@
       <c r="W162" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X162" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X162" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A163" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B163" s="11">
         <v>233353</v>
@@ -13211,13 +13208,13 @@
       <c r="W163" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X163" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X163" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A164" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B164" s="11">
         <v>233354</v>
@@ -13285,13 +13282,13 @@
       <c r="W164" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X164" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X164" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A165" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B165" s="11">
         <v>233355</v>
@@ -13359,13 +13356,13 @@
       <c r="W165" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X165" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X165" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A166" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B166" s="11">
         <v>233368</v>
@@ -13433,13 +13430,13 @@
       <c r="W166" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X166" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X166" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A167" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B167" s="11">
         <v>233356</v>
@@ -13507,13 +13504,13 @@
       <c r="W167" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X167" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X167" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A168" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B168" s="11">
         <v>233357</v>
@@ -13581,13 +13578,13 @@
       <c r="W168" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X168" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X168" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A169" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B169" s="11">
         <v>233358</v>
@@ -13655,13 +13652,13 @@
       <c r="W169" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X169" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="X169" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A170" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B170" s="11">
         <v>233359</v>
@@ -13727,15 +13724,15 @@
         <v>22</v>
       </c>
       <c r="W170" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X170" s="7">
         <v>8.18</v>
       </c>
     </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A171" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B171" s="11">
         <v>233360</v>
@@ -13801,15 +13798,15 @@
         <v>23</v>
       </c>
       <c r="W171" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X171" s="7">
         <v>7.14</v>
       </c>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A172" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B172" s="11">
         <v>233361</v>
@@ -13875,15 +13872,15 @@
         <v>23</v>
       </c>
       <c r="W172" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X172" s="7">
         <v>7.82</v>
       </c>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A173" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B173" s="11">
         <v>233362</v>
@@ -13951,8 +13948,8 @@
       <c r="W173" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="X173" s="7" t="s">
-        <v>13</v>
+      <c r="X173" s="7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>